<commit_message>
completed analysis before testing LL84 file
</commit_message>
<xml_diff>
--- a/data-files/berdo_data_files/berdo_building_summary_statistics.xlsx
+++ b/data-files/berdo_data_files/berdo_building_summary_statistics.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,16 @@
           <t>percentage_of_total_ghg</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>percent_of_city_wide_ghg</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>percent_of_building_sector_ghg</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -546,6 +556,12 @@
       <c r="G2" t="n">
         <v>4.521198108741022</v>
       </c>
+      <c r="H2" t="n">
+        <v>0.01365962312198423</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0196454632843102</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -571,6 +587,12 @@
       <c r="G3" t="n">
         <v>5.78847750255303</v>
       </c>
+      <c r="H3" t="n">
+        <v>0.01748837791073402</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.02515203260582779</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -596,6 +618,12 @@
       <c r="G4" t="n">
         <v>3.345318242326579</v>
       </c>
+      <c r="H4" t="n">
+        <v>0.01010700821203438</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01453604224439979</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -621,6 +649,12 @@
       <c r="G5" t="n">
         <v>1.177366037591638</v>
       </c>
+      <c r="H5" t="n">
+        <v>0.003557104989279935</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.005115878735546293</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -646,6 +680,12 @@
       <c r="G6" t="n">
         <v>17.06310282818375</v>
       </c>
+      <c r="H6" t="n">
+        <v>0.05155172330848289</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0741424180195539</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -671,6 +711,12 @@
       <c r="G7" t="n">
         <v>6.899602767675353</v>
       </c>
+      <c r="H7" t="n">
+        <v>0.02084535364987324</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.02998008262160302</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -696,6 +742,12 @@
       <c r="G8" t="n">
         <v>3.830871596933392</v>
       </c>
+      <c r="H8" t="n">
+        <v>0.01157398127316199</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.01664586366143962</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -721,6 +773,12 @@
       <c r="G9" t="n">
         <v>19.89478969616292</v>
       </c>
+      <c r="H9" t="n">
+        <v>0.06010692803204633</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.08644663452579296</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -746,6 +804,12 @@
       <c r="G10" t="n">
         <v>20.56568982758291</v>
       </c>
+      <c r="H10" t="n">
+        <v>0.06213387812962538</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.08936182284142298</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -771,6 +835,12 @@
       <c r="G11" t="n">
         <v>1.044088329522366</v>
       </c>
+      <c r="H11" t="n">
+        <v>0.00315444108935739</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.004536761816199221</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -796,6 +866,12 @@
       <c r="G12" t="n">
         <v>1.181453008328928</v>
       </c>
+      <c r="H12" t="n">
+        <v>0.003569452707437656</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.005133637398544989</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -821,6 +897,12 @@
       <c r="G13" t="n">
         <v>1.995078650301799</v>
       </c>
+      <c r="H13" t="n">
+        <v>0.006027610780680472</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.008668995127207379</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -846,6 +928,12 @@
       <c r="G14" t="n">
         <v>1.253426155338857</v>
       </c>
+      <c r="H14" t="n">
+        <v>0.003786900834994395</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.005446374372911627</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -870,6 +958,12 @@
       </c>
       <c r="G15" t="n">
         <v>11.43953724875746</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.03456158384341169</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.04970695899732282</v>
       </c>
     </row>
   </sheetData>
@@ -2204,285 +2298,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005983132403D1464F8DDC272820BA8C1B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fe6f55e11da51139aa85f6a00701c7d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4fe9914-c092-4200-a7d8-cc85a6bef288" xmlns:ns3="afc29c3b-9522-4360-ba9d-c1dc5ac90a19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="285f550d8d1fc9956465dc5fad4d328f" ns2:_="" ns3:_="">
-    <xsd:import namespace="d4fe9914-c092-4200-a7d8-cc85a6bef288"/>
-    <xsd:import namespace="afc29c3b-9522-4360-ba9d-c1dc5ac90a19"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d4fe9914-c092-4200-a7d8-cc85a6bef288" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a9be0bb2-3812-4b91-a213-01a8a1cc323e" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="afc29c3b-9522-4360-ba9d-c1dc5ac90a19" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{b3bae1d6-1973-4eec-951a-e9b4547540f9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="afc29c3b-9522-4360-ba9d-c1dc5ac90a19">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="afc29c3b-9522-4360-ba9d-c1dc5ac90a19" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d4fe9914-c092-4200-a7d8-cc85a6bef288">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4FD34B0-58DD-4B68-8097-7EBFE64E28AA}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B775AEA9-199E-46EB-8A7B-E59C9209F46C}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3931437-4BE8-4E28-8D7B-68F44DAA095C}"/>
 </file>
</xml_diff>